<commit_message>
Updated summary report formatting
</commit_message>
<xml_diff>
--- a/unit_tester/test_files/program/complex_cases.xlsx
+++ b/unit_tester/test_files/program/complex_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brt.hawayda\Desktop\42\minishell-jnde\unit_tester\test_files\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BC3D1F-F189-4C00-AC3E-C85089B53079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F70548-208F-4BCC-8E9E-C98E65085FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>$&gt;echo 'Hello World' | grep Hello &amp;&amp; cat &lt; input.txt &gt;&gt; output.txt</t>
+    <t>$&gt; echo 'Hello World' | grep Hello &amp;&amp; cat &lt; input.txt &gt;&gt; output.txt</t>
   </si>
 </sst>
 </file>
@@ -347,9 +347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>